<commit_message>
Added some more results from tweaking the model
</commit_message>
<xml_diff>
--- a/src/pytorch/results/Results - Tweaking Parameters (1st Model).xlsx
+++ b/src/pytorch/results/Results - Tweaking Parameters (1st Model).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luc\Documents\CPS 803\Main Project\src\pytorch\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDDF2FB-D648-4643-B9EC-8B4C79FA052C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9449C2-5178-4982-BD6B-8700F750C7F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +529,7 @@
         <v>0.75</v>
       </c>
       <c r="E5" s="1">
-        <v>61.45</v>
+        <v>0.61450000000000005</v>
       </c>
       <c r="F5" s="1">
         <v>0.86019999999999996</v>

</xml_diff>